<commit_message>
troubleshoot system process model
</commit_message>
<xml_diff>
--- a/exposan/enviroloo/data/units_data/bsm2p_init.xlsx
+++ b/exposan/enviroloo/data/units_data/bsm2p_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhpuri/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\enviroloo\data\units_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CA0F17-23E9-9942-94F4-27605F6F7F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B487466-0AF2-4AA5-9BF1-AEA341DCE4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26020" windowHeight="17320" activeTab="7" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="2910" yWindow="3765" windowWidth="40560" windowHeight="15990" activeTab="7" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="asm" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="72">
   <si>
     <t>S_O2</t>
   </si>
@@ -651,14 +651,14 @@
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="33" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -940,7 +940,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="21:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="21:26" x14ac:dyDescent="0.25">
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -1627,14 +1627,14 @@
       <selection activeCell="A8" activeCellId="3" sqref="A1:XFD1 A2:XFD2 A4:XFD4 A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="33" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -1821,132 +1821,132 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2">
         <f ca="1">asm!B3*(0.9+0.2*RAND())</f>
-        <v>1.8103437611799816E-2</v>
+        <v>1.8129295442659246E-2</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">asm!G3*(0.9+0.2*RAND())</f>
-        <v>0.21115542354760883</v>
+        <v>0.18267600081432717</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">asm!F3*(0.9+0.2*RAND())</f>
-        <v>36.796894866705003</v>
+        <v>37.658762109673063</v>
       </c>
       <c r="E3" s="2">
         <f ca="1">asm!H3*(0.9+0.2*RAND())</f>
-        <v>8.4232887940038345E-2</v>
+        <v>8.4979904287491859E-2</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">asm!I3*(0.9+0.2*RAND())</f>
-        <v>14.370707935183386</v>
+        <v>14.585159090501586</v>
       </c>
       <c r="G3" s="2">
         <f ca="1">asm!C3*(0.9+0.2*RAND())</f>
-        <v>76.127340399159763</v>
+        <v>74.992674885186858</v>
       </c>
       <c r="H3" s="2">
         <f ca="1">asm!D3*(0.9+0.2*RAND())</f>
-        <v>56.62296991195204</v>
+        <v>59.976786850010811</v>
       </c>
       <c r="I3" s="2">
         <f ca="1">asm!E3*(0.9+0.2*RAND())</f>
-        <v>28.942000805622914</v>
+        <v>26.755516572973637</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">asm!J3*(0.9+0.2*RAND())</f>
-        <v>84.498322170143098</v>
+        <v>82.298236936652103</v>
       </c>
       <c r="K3" s="2">
         <f ca="1">asm!R3*(0.9+0.2*RAND())</f>
-        <v>24.082782061770487</v>
+        <v>26.599734153518163</v>
       </c>
       <c r="L3" s="2">
         <f ca="1">asm!S3*(0.9+0.2*RAND())</f>
-        <v>101.63470714500032</v>
+        <v>94.169336907907038</v>
       </c>
       <c r="M3" s="2">
         <f ca="1">asm!K3*(0.9+0.2*RAND())</f>
-        <v>49.507344418840745</v>
+        <v>52.505385190076758</v>
       </c>
       <c r="N3" s="2">
         <f ca="1">asm!L3*(0.9+0.2*RAND())</f>
-        <v>213.02272199682042</v>
+        <v>214.67729794636844</v>
       </c>
       <c r="O3" s="2">
         <f ca="1">asm!M3*(0.9+0.2*RAND())</f>
-        <v>30.564502952914335</v>
+        <v>30.099450976386034</v>
       </c>
       <c r="P3" s="2">
         <f ca="1">asm!N3*(0.9+0.2*RAND())</f>
-        <v>0.47563540524101666</v>
+        <v>0.49737259276704782</v>
       </c>
       <c r="Q3" s="2">
         <f ca="1">asm!O3*(0.9+0.2*RAND())</f>
-        <v>0.13006400133053719</v>
+        <v>0.12730959755547203</v>
       </c>
       <c r="R3" s="2">
         <f ca="1">asm!P3*(0.9+0.2*RAND())</f>
-        <v>3.1658210830036031E-4</v>
+        <v>2.9454998042642729E-4</v>
       </c>
       <c r="S3" s="2">
         <f ca="1">asm!Q3*(0.9+0.2*RAND())</f>
-        <v>4.9339835051779128E-2</v>
+        <v>5.7791737826242917E-2</v>
       </c>
       <c r="T3" s="2">
         <f ca="1">asm!V3*(0.9+0.2*RAND())</f>
-        <v>119.72967660444071</v>
+        <v>108.38551583667018</v>
       </c>
       <c r="U3" s="2">
         <f ca="1">asm!W3*(0.9+0.2*RAND())</f>
-        <v>1.046361208189612E-5</v>
+        <v>1.0036088395733994E-5</v>
       </c>
       <c r="V3" s="2">
         <f ca="1">asm!X3*(0.9+0.2*RAND())</f>
-        <v>1.0560198889429461E-5</v>
+        <v>1.047504190201383E-5</v>
       </c>
       <c r="W3" s="2">
         <f ca="1">asm!Y3*(0.9+0.2*RAND())</f>
-        <v>1.0995034386005718E-5</v>
+        <v>9.428476315257217E-6</v>
       </c>
       <c r="X3" s="2">
         <f ca="1">asm!Z3*(0.9+0.2*RAND())</f>
-        <v>9.1876095110479296E-6</v>
+        <v>9.7763076879276124E-6</v>
       </c>
       <c r="Y3" s="2">
         <f ca="1">asm!AA3*(0.9+0.2*RAND())</f>
-        <v>9.0702248348508032E-6</v>
+        <v>1.0810625011782534E-5</v>
       </c>
       <c r="Z3" s="2">
         <f ca="1">asm!AB3*(0.9+0.2*RAND())</f>
-        <v>9.4479871013495431E-6</v>
+        <v>1.0565848264027958E-5</v>
       </c>
       <c r="AA3" s="2">
         <f ca="1">asm!AC3*(0.9+0.2*RAND())</f>
-        <v>9.2464927082655827E-6</v>
+        <v>9.6220928057620398E-6</v>
       </c>
       <c r="AB3" s="2">
         <f ca="1">asm!AD3*(0.9+0.2*RAND())</f>
-        <v>1.0583256479244435E-5</v>
+        <v>1.0974092013536752E-5</v>
       </c>
       <c r="AC3" s="2">
         <f ca="1">asm!AE3*(0.9+0.2*RAND())</f>
-        <v>1.0312995346566433E-5</v>
+        <v>1.0063667976543204E-5</v>
       </c>
       <c r="AD3" s="2">
         <f ca="1">asm!T3*(0.9+0.2*RAND())</f>
-        <v>74.555659503873699</v>
+        <v>79.371894623372398</v>
       </c>
       <c r="AE3" s="2">
         <f ca="1">asm!U3*(0.9+0.2*RAND())</f>
-        <v>464.08633585280376</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <v>461.50429951644628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>299.92681718591899</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>299.92681710062402</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>299.92681643170999</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>299.926816379716</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>299.92681627556999</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>299.92681617126402</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>299.92681606679997</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -2619,7 +2619,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -2630,7 +2630,7 @@
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -2642,7 +2642,7 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="21:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -2653,7 +2653,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -2664,7 +2664,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -2675,7 +2675,7 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -2686,7 +2686,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -2710,14 +2710,14 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="33" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -2904,132 +2904,132 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2">
         <f ca="1">asm!B3*(0.9+0.2*RAND())</f>
-        <v>1.7165702606329821E-2</v>
+        <v>1.5329370017016451E-2</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">asm!G3*(0.9+0.2*RAND())</f>
-        <v>0.20643010912856338</v>
+        <v>0.20423597648494976</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">asm!F3*(0.9+0.2*RAND())</f>
-        <v>33.887037779999723</v>
+        <v>34.086913773675825</v>
       </c>
       <c r="E3" s="2">
         <f ca="1">asm!H3*(0.9+0.2*RAND())</f>
-        <v>8.7749230030835346E-2</v>
+        <v>7.8310487776575496E-2</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">asm!I3*(0.9+0.2*RAND())</f>
-        <v>14.015286538082702</v>
+        <v>13.641924311295396</v>
       </c>
       <c r="G3" s="2">
         <f ca="1">asm!C3*(0.9+0.2*RAND())</f>
-        <v>75.046107386296242</v>
+        <v>67.251540009813539</v>
       </c>
       <c r="H3" s="2">
         <f ca="1">asm!D3*(0.9+0.2*RAND())</f>
-        <v>53.163578864739598</v>
+        <v>52.854276116420351</v>
       </c>
       <c r="I3" s="2">
         <f ca="1">asm!E3*(0.9+0.2*RAND())</f>
-        <v>26.923422510275351</v>
+        <v>28.14096367292483</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">asm!J3*(0.9+0.2*RAND())</f>
-        <v>84.253037928919781</v>
+        <v>84.390435091594554</v>
       </c>
       <c r="K3" s="2">
         <f ca="1">asm!R3*(0.9+0.2*RAND())</f>
-        <v>23.766048292122687</v>
+        <v>26.636191591201008</v>
       </c>
       <c r="L3" s="2">
         <f ca="1">asm!S3*(0.9+0.2*RAND())</f>
-        <v>104.73095806555369</v>
+        <v>103.17572232153776</v>
       </c>
       <c r="M3" s="2">
         <f ca="1">asm!K3*(0.9+0.2*RAND())</f>
-        <v>53.345868245296543</v>
+        <v>52.628472899145848</v>
       </c>
       <c r="N3" s="2">
         <f ca="1">asm!L3*(0.9+0.2*RAND())</f>
-        <v>217.74524250586336</v>
+        <v>224.40516370571757</v>
       </c>
       <c r="O3" s="2">
         <f ca="1">asm!M3*(0.9+0.2*RAND())</f>
-        <v>34.402852715893431</v>
+        <v>29.409899047372722</v>
       </c>
       <c r="P3" s="2">
         <f ca="1">asm!N3*(0.9+0.2*RAND())</f>
-        <v>0.44339526780219823</v>
+        <v>0.46303755598161905</v>
       </c>
       <c r="Q3" s="2">
         <f ca="1">asm!O3*(0.9+0.2*RAND())</f>
-        <v>0.15283874851522031</v>
+        <v>0.15253311415756685</v>
       </c>
       <c r="R3" s="2">
         <f ca="1">asm!P3*(0.9+0.2*RAND())</f>
-        <v>3.1192497055825523E-4</v>
+        <v>3.1843114526383762E-4</v>
       </c>
       <c r="S3" s="2">
         <f ca="1">asm!Q3*(0.9+0.2*RAND())</f>
-        <v>5.3434885267512666E-2</v>
+        <v>4.8924771953512497E-2</v>
       </c>
       <c r="T3" s="2">
         <f ca="1">asm!V3*(0.9+0.2*RAND())</f>
-        <v>110.66275653694102</v>
+        <v>120.70759144772616</v>
       </c>
       <c r="U3" s="2">
         <f ca="1">asm!W3*(0.9+0.2*RAND())</f>
-        <v>9.435618833401408E-6</v>
+        <v>1.0338986438960643E-5</v>
       </c>
       <c r="V3" s="2">
         <f ca="1">asm!X3*(0.9+0.2*RAND())</f>
-        <v>1.0295776070995012E-5</v>
+        <v>9.6173003885338793E-6</v>
       </c>
       <c r="W3" s="2">
         <f ca="1">asm!Y3*(0.9+0.2*RAND())</f>
-        <v>1.0225790234278494E-5</v>
+        <v>1.0749924406027423E-5</v>
       </c>
       <c r="X3" s="2">
         <f ca="1">asm!Z3*(0.9+0.2*RAND())</f>
-        <v>9.922219852908708E-6</v>
+        <v>1.097650465546533E-5</v>
       </c>
       <c r="Y3" s="2">
         <f ca="1">asm!AA3*(0.9+0.2*RAND())</f>
-        <v>1.0061031188360063E-5</v>
+        <v>1.062360291633105E-5</v>
       </c>
       <c r="Z3" s="2">
         <f ca="1">asm!AB3*(0.9+0.2*RAND())</f>
-        <v>1.0053897247861018E-5</v>
+        <v>9.3163345204359746E-6</v>
       </c>
       <c r="AA3" s="2">
         <f ca="1">asm!AC3*(0.9+0.2*RAND())</f>
-        <v>9.0539893066532437E-6</v>
+        <v>9.1692101752390814E-6</v>
       </c>
       <c r="AB3" s="2">
         <f ca="1">asm!AD3*(0.9+0.2*RAND())</f>
-        <v>1.053255266033707E-5</v>
+        <v>9.8201878225313595E-6</v>
       </c>
       <c r="AC3" s="2">
         <f ca="1">asm!AE3*(0.9+0.2*RAND())</f>
-        <v>1.0731422301699087E-5</v>
+        <v>1.0608340796533643E-5</v>
       </c>
       <c r="AD3" s="2">
         <f ca="1">asm!T3*(0.9+0.2*RAND())</f>
-        <v>79.166004615005932</v>
+        <v>84.638303665601754</v>
       </c>
       <c r="AE3" s="2">
         <f ca="1">asm!U3*(0.9+0.2*RAND())</f>
-        <v>450.06325558911107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <v>417.53087988060901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>299.91253823298899</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>299.91253759370102</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>299.89821486787002</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>299.89821451696002</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>299.89821377600401</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>299.89821304423799</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>299.89821230976298</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -3715,9 +3715,9 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -3938,9 +3938,9 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -4216,9 +4216,9 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>118.9924</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>140.10169999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -4404,9 +4404,9 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>52</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1.641</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>14.91</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>17</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G6">
         <v>21325.5088</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G7">
         <v>41771.508800000003</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G8">
         <v>41771.508800000003</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>103109.5088</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G10">
         <v>103109.5088</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G11">
         <v>103109.5088</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G12">
         <v>103109.5088</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>15.096</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G13">
         <v>103109.5088</v>
       </c>
@@ -4525,15 +4525,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BCF21F6-DF53-C943-85F5-5A46E588E886}">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4625,199 +4625,199 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>25.19</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5.6520000000000001</v>
-      </c>
-      <c r="G2" s="2">
-        <v>70</v>
-      </c>
-      <c r="H2" s="2">
-        <v>57.45</v>
-      </c>
-      <c r="I2" s="2">
-        <v>26.6</v>
-      </c>
-      <c r="J2" s="2">
-        <v>84</v>
-      </c>
-      <c r="K2" s="2">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>3.0474042058124102E-3</v>
+      </c>
+      <c r="C2">
+        <v>11.714418849847901</v>
+      </c>
+      <c r="D2">
+        <v>18.8903691863988</v>
+      </c>
+      <c r="E2">
+        <v>0.11946083149644</v>
+      </c>
+      <c r="F2">
+        <v>13.9810263597446</v>
+      </c>
+      <c r="G2">
+        <v>6.5555411612357402</v>
+      </c>
+      <c r="H2">
+        <v>24.574442076447799</v>
+      </c>
+      <c r="I2">
+        <v>26.593511091194799</v>
+      </c>
+      <c r="J2">
+        <v>46.417063153684701</v>
+      </c>
+      <c r="K2">
+        <v>23.325330665950201</v>
+      </c>
+      <c r="L2">
+        <v>30.394208886020799</v>
+      </c>
+      <c r="M2">
+        <v>1192.9927654390001</v>
+      </c>
+      <c r="N2">
+        <v>106.103655323589</v>
+      </c>
+      <c r="O2">
+        <v>1587.47408876292</v>
+      </c>
+      <c r="P2">
+        <v>326.15633508048103</v>
+      </c>
+      <c r="Q2">
+        <v>93.018247423488702</v>
+      </c>
+      <c r="R2">
+        <v>14.8592292888102</v>
+      </c>
+      <c r="S2">
+        <v>86.981310436304597</v>
+      </c>
+      <c r="T2">
+        <v>59.759826732459601</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD2">
+        <v>174.957309519863</v>
+      </c>
+      <c r="AE2">
+        <v>299.92681718591899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="2">
-        <v>94.1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>370</v>
-      </c>
-      <c r="O2" s="2">
-        <v>51.53</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>60</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>175</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
       <c r="B3">
-        <v>3.0474042058124102E-3</v>
+        <v>3.4087014628173198</v>
       </c>
       <c r="C3">
-        <v>11.714418849847901</v>
+        <v>14.562662155920901</v>
       </c>
       <c r="D3">
-        <v>18.8903691863988</v>
+        <v>2.80396789146217</v>
       </c>
       <c r="E3">
-        <v>0.11946083149644</v>
+        <v>5.7703053500929702</v>
       </c>
       <c r="F3">
-        <v>13.9810263597446</v>
+        <v>5.7663022533402604</v>
       </c>
       <c r="G3">
-        <v>6.5555411612357402</v>
+        <v>0.31053079106644299</v>
       </c>
       <c r="H3">
-        <v>24.574442076447799</v>
+        <v>1.8683680536395599E-2</v>
       </c>
       <c r="I3">
-        <v>26.593511091194799</v>
+        <v>26.5935110101913</v>
       </c>
       <c r="J3">
-        <v>46.417063153684701</v>
+        <v>3.1527118926041999</v>
       </c>
       <c r="K3">
-        <v>23.325330665950201</v>
+        <v>20.0333521904004</v>
       </c>
       <c r="L3">
-        <v>30.394208886020799</v>
+        <v>28.3477546584907</v>
       </c>
       <c r="M3">
-        <v>1192.9927654390001</v>
+        <v>1202.16848045137</v>
       </c>
       <c r="N3">
-        <v>106.103655323589</v>
+        <v>36.326993213211701</v>
       </c>
       <c r="O3">
-        <v>1587.47408876292</v>
+        <v>1605.9559534970899</v>
       </c>
       <c r="P3">
-        <v>326.15633508048103</v>
+        <v>336.75178105965301</v>
       </c>
       <c r="Q3">
-        <v>93.018247423488702</v>
+        <v>100.92055904562601</v>
       </c>
       <c r="R3">
-        <v>14.8592292888102</v>
+        <v>2.9556009152170102</v>
       </c>
       <c r="S3">
-        <v>86.981310436304597</v>
+        <v>89.364440513125004</v>
       </c>
       <c r="T3">
-        <v>59.759826732459601</v>
-      </c>
-      <c r="U3">
-        <v>3.2343485435841597E-2</v>
+        <v>59.759548692966199</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="V3" s="1">
-        <v>4.9248224056000201E-9</v>
-      </c>
-      <c r="W3">
-        <v>0.56676361511683904</v>
+        <v>1E-8</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="X3" s="1">
-        <v>2.5741800565300101E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
-        <v>2.91456298717996E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="Z3" s="1">
-        <v>2.9116388217527898E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AA3" s="1">
-        <v>2.9128622440031698E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AB3" s="1">
-        <v>2.91438458769372E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AC3" s="1">
-        <v>2.4790217734229101E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="AD3">
-        <v>174.957309519863</v>
+        <v>174.95730898241101</v>
       </c>
       <c r="AE3">
-        <v>299.92681718591899</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <v>299.92681627556999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>3.4087014628173198</v>
@@ -4876,132 +4876,37 @@
       <c r="T4">
         <v>59.759548692966199</v>
       </c>
-      <c r="U4">
-        <v>3.2471843306945497E-2</v>
+      <c r="U4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="V4" s="1">
-        <v>4.9906484593148497E-9</v>
-      </c>
-      <c r="W4">
-        <v>0.56672240226555604</v>
+        <v>1E-8</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="X4" s="1">
-        <v>2.62794444062592E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
-        <v>2.9559638006753001E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="Z4" s="1">
-        <v>2.9530395905932002E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AA4" s="1">
-        <v>2.9542631088832099E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AB4" s="1">
-        <v>2.9557853498085E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="AC4" s="1">
-        <v>2.51267015214776E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="AD4">
         <v>174.95730898241101</v>
       </c>
       <c r="AE4">
-        <v>299.92681627556999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5">
-        <v>3.4087014628173198</v>
-      </c>
-      <c r="C5">
-        <v>14.562662155920901</v>
-      </c>
-      <c r="D5">
-        <v>2.80396789146217</v>
-      </c>
-      <c r="E5">
-        <v>5.7703053500929702</v>
-      </c>
-      <c r="F5">
-        <v>5.7663022533402604</v>
-      </c>
-      <c r="G5">
-        <v>0.31053079106644299</v>
-      </c>
-      <c r="H5">
-        <v>1.8683680536395599E-2</v>
-      </c>
-      <c r="I5">
-        <v>26.5935110101913</v>
-      </c>
-      <c r="J5">
-        <v>3.1527118926041999</v>
-      </c>
-      <c r="K5">
-        <v>20.0333521904004</v>
-      </c>
-      <c r="L5">
-        <v>28.3477546584907</v>
-      </c>
-      <c r="M5">
-        <v>1202.16848045137</v>
-      </c>
-      <c r="N5">
-        <v>36.326993213211701</v>
-      </c>
-      <c r="O5">
-        <v>1605.9559534970899</v>
-      </c>
-      <c r="P5">
-        <v>336.75178105965301</v>
-      </c>
-      <c r="Q5">
-        <v>100.92055904562601</v>
-      </c>
-      <c r="R5">
-        <v>2.9556009152170102</v>
-      </c>
-      <c r="S5">
-        <v>89.364440513125004</v>
-      </c>
-      <c r="T5">
-        <v>59.759548692966199</v>
-      </c>
-      <c r="U5">
-        <v>3.2471843306945497E-2</v>
-      </c>
-      <c r="V5" s="1">
-        <v>4.9906484593148497E-9</v>
-      </c>
-      <c r="W5">
-        <v>0.56672240226555604</v>
-      </c>
-      <c r="X5" s="1">
-        <v>2.62794444062592E-13</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>2.9559638006753001E-12</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>2.9530395905932002E-12</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>2.9542631088832099E-12</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>2.9557853498085E-12</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>2.51267015214776E-11</v>
-      </c>
-      <c r="AD5">
-        <v>174.95730898241101</v>
-      </c>
-      <c r="AE5">
         <v>299.92681627556999</v>
       </c>
     </row>

</xml_diff>